<commit_message>
fixed the hyperlink issue
</commit_message>
<xml_diff>
--- a/FOLDER/FINESTAR/FINESTAR_21_01_2025_04_39_52487.xlsx
+++ b/FOLDER/FINESTAR/FINESTAR_21_01_2025_04_39_52487.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3501" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3452" uniqueCount="236">
   <si>
     <t>SrNo</t>
   </si>
@@ -735,54 +735,6 @@
   </si>
   <si>
     <t>1014045802</t>
-  </si>
-  <si>
-    <t>All Parameter Summary</t>
-  </si>
-  <si>
-    <t>Pcs</t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Color</t>
-  </si>
-  <si>
-    <t>Cut</t>
-  </si>
-  <si>
-    <t>Flour</t>
-  </si>
-  <si>
-    <t>Note.</t>
-  </si>
-  <si>
-    <t>(1) RAP PRICE MENTION IN LIST MAY BE CHANGE</t>
-  </si>
-  <si>
-    <t>(2) RAP PRICE WILL BE TAKEN AS OF DATE OF SALE</t>
-  </si>
-  <si>
-    <t>(3) PLEASE CHECK DAILY UPDATED PRICE</t>
-  </si>
-  <si>
-    <t>(4) BOLD IS NEW GOODS UPDATED</t>
-  </si>
-  <si>
-    <t>Finestar Jewellery &amp; Diamonds Pvt. Ltd.</t>
-  </si>
-  <si>
-    <t>ESTIMATED LIST (21-01-2025 10:09:52)</t>
-  </si>
-  <si>
-    <t>DE-6010, D-TOWER, BHARAT DIAMOND BOURSE, BANDRA-KURLA COMPLEX, BANDRA (E),  MUMBAI - 400 051, MAHARASHTRA, INDIA</t>
-  </si>
-  <si>
-    <t>Website Name:www.finestardiamonds.com/Email Id :sales@finestardiamonds.com</t>
   </si>
 </sst>
 </file>
@@ -796,7 +748,7 @@
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="180" formatCode="#,##0.00;"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -826,42 +778,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="22"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1211,7 +1127,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1276,21 +1192,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1395,152 +1296,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1563,24 +1464,6 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1964,10 +1847,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:BC149"/>
+  <dimension ref="A1:BA104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD2"/>
+    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="67" topLeftCell="A129" workbookViewId="0">
+      <selection activeCell="A150" sqref="$A105:$XFD150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -18736,1009 +18619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:52">
-      <c r="A105" s="3"/>
-      <c r="B105" s="3"/>
-      <c r="C105" s="3"/>
-      <c r="D105" s="3"/>
-      <c r="E105" s="3"/>
-      <c r="F105" s="3"/>
-      <c r="G105" s="3"/>
-      <c r="H105" s="8">
-        <f ca="1">ROUND(SUMPRODUCT((BA2:BA104=1)*(SUBTOTAL(9,OFFSET(H2,ROW(H2:H104)-ROW(H2),0)))),2)</f>
-        <v>49.69</v>
-      </c>
-      <c r="I105" s="3"/>
-      <c r="J105" s="3"/>
-      <c r="K105" s="3"/>
-      <c r="L105" s="3"/>
-      <c r="M105" s="8"/>
-      <c r="N105" s="8"/>
-      <c r="O105" s="3"/>
-      <c r="P105" s="3"/>
-      <c r="Q105" s="3"/>
-      <c r="R105" s="3"/>
-      <c r="S105" s="3"/>
-      <c r="T105" s="3"/>
-      <c r="U105" s="3"/>
-      <c r="V105" s="3"/>
-      <c r="W105" s="3"/>
-      <c r="X105" s="3"/>
-      <c r="Y105" s="3"/>
-      <c r="Z105" s="3"/>
-      <c r="AA105" s="3"/>
-      <c r="AB105" s="3"/>
-      <c r="AC105" s="3"/>
-      <c r="AD105" s="3"/>
-      <c r="AE105" s="3"/>
-      <c r="AF105" s="3"/>
-      <c r="AG105" s="3"/>
-      <c r="AH105" s="3"/>
-      <c r="AI105" s="3"/>
-      <c r="AJ105" s="3"/>
-      <c r="AK105" s="3"/>
-      <c r="AL105" s="3"/>
-      <c r="AM105" s="3"/>
-      <c r="AN105" s="3"/>
-      <c r="AO105" s="3"/>
-      <c r="AP105" s="3"/>
-      <c r="AQ105" s="3"/>
-      <c r="AR105" s="3"/>
-      <c r="AS105" s="3"/>
-      <c r="AT105" s="3"/>
-      <c r="AU105" s="3"/>
-      <c r="AV105" s="3"/>
-      <c r="AW105" s="3"/>
-      <c r="AX105" s="3"/>
-      <c r="AY105" s="3"/>
-      <c r="AZ105" s="3">
-        <f ca="1">ROUND(SUMPRODUCT((BA2:BA104=1)*(SUBTOTAL(9,OFFSET(AZ2,ROW(AZ2:AZ104)-ROW(AZ2),0)))),2)</f>
-        <v>130566</v>
-      </c>
-    </row>
-    <row r="107" ht="18" spans="2:17">
-      <c r="B107" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="C107" s="9"/>
-      <c r="D107" s="9"/>
-      <c r="E107" s="9"/>
-      <c r="F107" s="9"/>
-      <c r="G107" s="9"/>
-      <c r="H107" s="9"/>
-      <c r="I107" s="9"/>
-      <c r="J107" s="9"/>
-      <c r="K107" s="9"/>
-      <c r="L107" s="9"/>
-      <c r="M107" s="9"/>
-      <c r="N107" s="9"/>
-      <c r="O107" s="9"/>
-      <c r="P107" s="9"/>
-      <c r="Q107" s="9"/>
-    </row>
-    <row r="108" spans="2:9">
-      <c r="B108" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C108" s="10"/>
-      <c r="D108" s="10"/>
-      <c r="G108" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H108" s="10"/>
-      <c r="I108" s="10"/>
-    </row>
-    <row r="109" spans="2:9">
-      <c r="B109" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C109" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="D109" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="G109" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H109" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="I109" s="11" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="110" spans="2:9">
-      <c r="B110" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C110" s="10">
-        <f ca="1">SUMPRODUCT(SUBTOTAL(3,OFFSET($G$2:$G$105,ROW($G$2:$G$105)-MIN(ROW($G$2:$G$105)),,1)),--($G$2:$G$105=B110))</f>
-        <v>103</v>
-      </c>
-      <c r="D110" s="12">
-        <f ca="1">C110/$C$116</f>
-        <v>1</v>
-      </c>
-      <c r="G110" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="H110" s="10">
-        <f ca="1">SUMPRODUCT(SUBTOTAL(3,OFFSET($J$2:$J$105,ROW($J$2:$J$105)-MIN(ROW($J$2:$J$105)),,1)),--($J$2:$J$105=G110),--($BA$2:$BA$105=1))</f>
-        <v>59</v>
-      </c>
-      <c r="I110" s="12">
-        <f ca="1">H110/$H$116</f>
-        <v>0.572815533980582</v>
-      </c>
-    </row>
-    <row r="111" spans="2:9">
-      <c r="B111" s="11"/>
-      <c r="C111" s="10"/>
-      <c r="D111" s="10"/>
-      <c r="G111" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="H111" s="10">
-        <f ca="1">SUMPRODUCT(SUBTOTAL(3,OFFSET($J$2:$J$105,ROW($J$2:$J$105)-MIN(ROW($J$2:$J$105)),,1)),--($J$2:$J$105=G111),--($BA$2:$BA$105=1))</f>
-        <v>21</v>
-      </c>
-      <c r="I111" s="12">
-        <f ca="1">H111/$H$116</f>
-        <v>0.203883495145631</v>
-      </c>
-    </row>
-    <row r="112" spans="2:9">
-      <c r="B112" s="11"/>
-      <c r="C112" s="10"/>
-      <c r="D112" s="10"/>
-      <c r="G112" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="H112" s="10">
-        <f ca="1">SUMPRODUCT(SUBTOTAL(3,OFFSET($J$2:$J$105,ROW($J$2:$J$105)-MIN(ROW($J$2:$J$105)),,1)),--($J$2:$J$105=G112),--($BA$2:$BA$105=1))</f>
-        <v>12</v>
-      </c>
-      <c r="I112" s="12">
-        <f ca="1">H112/$H$116</f>
-        <v>0.116504854368932</v>
-      </c>
-    </row>
-    <row r="113" spans="2:9">
-      <c r="B113" s="11"/>
-      <c r="C113" s="10"/>
-      <c r="D113" s="10"/>
-      <c r="G113" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="H113" s="10">
-        <f ca="1">SUMPRODUCT(SUBTOTAL(3,OFFSET($J$2:$J$105,ROW($J$2:$J$105)-MIN(ROW($J$2:$J$105)),,1)),--($J$2:$J$105=G113),--($BA$2:$BA$105=1))</f>
-        <v>7</v>
-      </c>
-      <c r="I113" s="12">
-        <f ca="1">H113/$H$116</f>
-        <v>0.0679611650485437</v>
-      </c>
-    </row>
-    <row r="114" spans="2:9">
-      <c r="B114" s="11"/>
-      <c r="C114" s="10"/>
-      <c r="D114" s="10"/>
-      <c r="G114" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="H114" s="10">
-        <f ca="1">SUMPRODUCT(SUBTOTAL(3,OFFSET($J$2:$J$105,ROW($J$2:$J$105)-MIN(ROW($J$2:$J$105)),,1)),--($J$2:$J$105=G114),--($BA$2:$BA$105=1))</f>
-        <v>4</v>
-      </c>
-      <c r="I114" s="12">
-        <f ca="1">H114/$H$116</f>
-        <v>0.0388349514563107</v>
-      </c>
-    </row>
-    <row r="115" spans="2:9">
-      <c r="B115" s="11"/>
-      <c r="C115" s="10"/>
-      <c r="D115" s="10"/>
-      <c r="G115" s="11"/>
-      <c r="H115" s="10"/>
-      <c r="I115" s="10"/>
-    </row>
-    <row r="116" spans="2:9">
-      <c r="B116" s="11" t="s">
-        <v>239</v>
-      </c>
-      <c r="C116" s="10">
-        <f ca="1">ROUND(SUM(C110:C115),2)</f>
-        <v>103</v>
-      </c>
-      <c r="D116" s="12">
-        <f ca="1">ROUND(SUM(D110:D115),2)</f>
-        <v>1</v>
-      </c>
-      <c r="G116" s="11" t="s">
-        <v>239</v>
-      </c>
-      <c r="H116" s="10">
-        <f ca="1">ROUND(SUM(H110:H115),2)</f>
-        <v>103</v>
-      </c>
-      <c r="I116" s="12">
-        <f ca="1">ROUND(SUM(I110:I115),2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="2:9">
-      <c r="B118" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="C118" s="10"/>
-      <c r="D118" s="10"/>
-      <c r="G118" s="10" t="s">
-        <v>241</v>
-      </c>
-      <c r="H118" s="10"/>
-      <c r="I118" s="10"/>
-    </row>
-    <row r="119" spans="2:9">
-      <c r="B119" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="C119" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="D119" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="G119" s="11" t="s">
-        <v>241</v>
-      </c>
-      <c r="H119" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="I119" s="11" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="120" spans="2:9">
-      <c r="B120" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C120" s="10">
-        <f ca="1">SUMPRODUCT(SUBTOTAL(3,OFFSET($I$2:$I$105,ROW($I$2:$I$105)-MIN(ROW($I$2:$I$105)),,1)),--($I$2:$I$105=B120),--($BA$2:$BA$105=1))</f>
-        <v>39</v>
-      </c>
-      <c r="D120" s="12">
-        <f ca="1" t="shared" ref="D120:D125" si="0">C120/$C$127</f>
-        <v>0.378640776699029</v>
-      </c>
-      <c r="G120" s="11"/>
-      <c r="H120" s="10"/>
-      <c r="I120" s="10"/>
-    </row>
-    <row r="121" spans="2:9">
-      <c r="B121" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C121" s="10">
-        <f ca="1">SUMPRODUCT(SUBTOTAL(3,OFFSET($I$2:$I$105,ROW($I$2:$I$105)-MIN(ROW($I$2:$I$105)),,1)),--($I$2:$I$105=B121),--($BA$2:$BA$105=1))</f>
-        <v>29</v>
-      </c>
-      <c r="D121" s="12">
-        <f ca="1" t="shared" si="0"/>
-        <v>0.281553398058252</v>
-      </c>
-      <c r="G121" s="11"/>
-      <c r="H121" s="10"/>
-      <c r="I121" s="10"/>
-    </row>
-    <row r="122" spans="2:9">
-      <c r="B122" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="C122" s="10">
-        <f ca="1">SUMPRODUCT(SUBTOTAL(3,OFFSET($I$2:$I$105,ROW($I$2:$I$105)-MIN(ROW($I$2:$I$105)),,1)),--($I$2:$I$105=B122),--($BA$2:$BA$105=1))</f>
-        <v>16</v>
-      </c>
-      <c r="D122" s="12">
-        <f ca="1" t="shared" si="0"/>
-        <v>0.155339805825243</v>
-      </c>
-      <c r="G122" s="11"/>
-      <c r="H122" s="10"/>
-      <c r="I122" s="10"/>
-    </row>
-    <row r="123" spans="2:9">
-      <c r="B123" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="C123" s="10">
-        <f ca="1">SUMPRODUCT(SUBTOTAL(3,OFFSET($I$2:$I$105,ROW($I$2:$I$105)-MIN(ROW($I$2:$I$105)),,1)),--($I$2:$I$105=B123),--($BA$2:$BA$105=1))</f>
-        <v>7</v>
-      </c>
-      <c r="D123" s="12">
-        <f ca="1" t="shared" si="0"/>
-        <v>0.0679611650485437</v>
-      </c>
-      <c r="G123" s="11"/>
-      <c r="H123" s="10"/>
-      <c r="I123" s="10"/>
-    </row>
-    <row r="124" spans="2:9">
-      <c r="B124" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C124" s="10">
-        <f ca="1">SUMPRODUCT(SUBTOTAL(3,OFFSET($I$2:$I$105,ROW($I$2:$I$105)-MIN(ROW($I$2:$I$105)),,1)),--($I$2:$I$105=B124),--($BA$2:$BA$105=1))</f>
-        <v>5</v>
-      </c>
-      <c r="D124" s="12">
-        <f ca="1" t="shared" si="0"/>
-        <v>0.0485436893203883</v>
-      </c>
-      <c r="G124" s="11"/>
-      <c r="H124" s="10"/>
-      <c r="I124" s="10"/>
-    </row>
-    <row r="125" spans="2:9">
-      <c r="B125" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C125" s="10">
-        <f ca="1">SUMPRODUCT(SUBTOTAL(3,OFFSET($I$2:$I$105,ROW($I$2:$I$105)-MIN(ROW($I$2:$I$105)),,1)),--($I$2:$I$105=B125),--($BA$2:$BA$105=1))</f>
-        <v>7</v>
-      </c>
-      <c r="D125" s="12">
-        <f ca="1" t="shared" si="0"/>
-        <v>0.0679611650485437</v>
-      </c>
-      <c r="G125" s="11"/>
-      <c r="H125" s="10"/>
-      <c r="I125" s="10"/>
-    </row>
-    <row r="126" spans="2:9">
-      <c r="B126" s="11"/>
-      <c r="C126" s="10"/>
-      <c r="D126" s="10"/>
-      <c r="G126" s="11"/>
-      <c r="H126" s="10"/>
-      <c r="I126" s="10"/>
-    </row>
-    <row r="127" spans="2:9">
-      <c r="B127" s="11" t="s">
-        <v>239</v>
-      </c>
-      <c r="C127" s="10">
-        <f ca="1">ROUND(SUM(C120:C126),2)</f>
-        <v>103</v>
-      </c>
-      <c r="D127" s="12">
-        <f ca="1">ROUND(SUM(D120:D126),2)</f>
-        <v>1</v>
-      </c>
-      <c r="G127" s="11" t="s">
-        <v>239</v>
-      </c>
-      <c r="H127" s="10">
-        <f>ROUND(SUM(H120:H126),2)</f>
-        <v>0</v>
-      </c>
-      <c r="I127" s="12">
-        <f>ROUND(SUM(I120:I126),2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="2:4">
-      <c r="B129" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="C129" s="10"/>
-      <c r="D129" s="10"/>
-    </row>
-    <row r="130" spans="2:4">
-      <c r="B130" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="C130" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="D130" s="11" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="131" spans="2:4">
-      <c r="B131" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C131" s="10">
-        <f ca="1">SUMPRODUCT(SUBTOTAL(3,OFFSET($R$2:$R$105,ROW($R$2:$R$105)-MIN(ROW($R$2:$R$105)),,1)),--($R$2:$R$105=B131),--($BA$2:$BA$105=1))</f>
-        <v>94</v>
-      </c>
-      <c r="D131" s="12">
-        <f ca="1">C131/$C$134</f>
-        <v>0.912621359223301</v>
-      </c>
-    </row>
-    <row r="132" spans="2:4">
-      <c r="B132" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="C132" s="10">
-        <f ca="1">SUMPRODUCT(SUBTOTAL(3,OFFSET($R$2:$R$105,ROW($R$2:$R$105)-MIN(ROW($R$2:$R$105)),,1)),--($R$2:$R$105=B132),--($BA$2:$BA$105=1))</f>
-        <v>9</v>
-      </c>
-      <c r="D132" s="12">
-        <f ca="1">C132/$C$134</f>
-        <v>0.087378640776699</v>
-      </c>
-    </row>
-    <row r="133" spans="2:4">
-      <c r="B133" s="11"/>
-      <c r="C133" s="10"/>
-      <c r="D133" s="10"/>
-    </row>
-    <row r="134" spans="2:4">
-      <c r="B134" s="11" t="s">
-        <v>239</v>
-      </c>
-      <c r="C134" s="10">
-        <f ca="1">ROUND(SUM(C131:C133),2)</f>
-        <v>103</v>
-      </c>
-      <c r="D134" s="12">
-        <f ca="1">ROUND(SUM(D131:D133),2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="138" spans="1:55">
-      <c r="A138" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="B138" s="13"/>
-      <c r="C138" s="13"/>
-      <c r="D138" s="13"/>
-      <c r="E138" s="13"/>
-      <c r="F138" s="13"/>
-      <c r="G138" s="13"/>
-      <c r="H138" s="13"/>
-      <c r="I138" s="13"/>
-      <c r="J138" s="13"/>
-      <c r="K138" s="13"/>
-      <c r="L138" s="13"/>
-      <c r="M138" s="13"/>
-      <c r="N138" s="13"/>
-      <c r="O138" s="13"/>
-      <c r="P138" s="13"/>
-      <c r="Q138" s="13"/>
-      <c r="R138" s="13"/>
-      <c r="S138" s="13"/>
-      <c r="T138" s="13"/>
-      <c r="U138" s="13"/>
-      <c r="V138" s="13"/>
-      <c r="W138" s="13"/>
-      <c r="X138" s="13"/>
-      <c r="Y138" s="13"/>
-      <c r="Z138" s="13"/>
-      <c r="AA138" s="13"/>
-      <c r="AB138" s="13"/>
-      <c r="AC138" s="13"/>
-      <c r="AD138" s="13"/>
-      <c r="AE138" s="13"/>
-      <c r="AF138" s="13"/>
-      <c r="AG138" s="13"/>
-      <c r="AH138" s="13"/>
-      <c r="AI138" s="13"/>
-      <c r="AJ138" s="13"/>
-      <c r="AK138" s="13"/>
-      <c r="AL138" s="13"/>
-      <c r="AM138" s="13"/>
-      <c r="AN138" s="13"/>
-      <c r="AO138" s="13"/>
-      <c r="AP138" s="13"/>
-      <c r="AQ138" s="13"/>
-      <c r="AR138" s="13"/>
-      <c r="AS138" s="13"/>
-      <c r="AT138" s="13"/>
-      <c r="AU138" s="13"/>
-      <c r="AV138" s="13"/>
-      <c r="AW138" s="13"/>
-      <c r="AX138" s="13"/>
-      <c r="AY138" s="13"/>
-      <c r="AZ138" s="13"/>
-      <c r="BA138" s="13"/>
-      <c r="BB138" s="13"/>
-      <c r="BC138" s="13"/>
-    </row>
-    <row r="139" spans="1:55">
-      <c r="A139" s="13" t="s">
-        <v>244</v>
-      </c>
-      <c r="B139" s="13"/>
-      <c r="C139" s="13"/>
-      <c r="D139" s="13"/>
-      <c r="E139" s="13"/>
-      <c r="F139" s="13"/>
-      <c r="G139" s="13"/>
-      <c r="H139" s="13"/>
-      <c r="I139" s="13"/>
-      <c r="J139" s="13"/>
-      <c r="K139" s="13"/>
-      <c r="L139" s="13"/>
-      <c r="M139" s="13"/>
-      <c r="N139" s="13"/>
-      <c r="O139" s="13"/>
-      <c r="P139" s="13"/>
-      <c r="Q139" s="13"/>
-      <c r="R139" s="13"/>
-      <c r="S139" s="13"/>
-      <c r="T139" s="13"/>
-      <c r="U139" s="13"/>
-      <c r="V139" s="13"/>
-      <c r="W139" s="13"/>
-      <c r="X139" s="13"/>
-      <c r="Y139" s="13"/>
-      <c r="Z139" s="13"/>
-      <c r="AA139" s="13"/>
-      <c r="AB139" s="13"/>
-      <c r="AC139" s="13"/>
-      <c r="AD139" s="13"/>
-      <c r="AE139" s="13"/>
-      <c r="AF139" s="13"/>
-      <c r="AG139" s="13"/>
-      <c r="AH139" s="13"/>
-      <c r="AI139" s="13"/>
-      <c r="AJ139" s="13"/>
-      <c r="AK139" s="13"/>
-      <c r="AL139" s="13"/>
-      <c r="AM139" s="13"/>
-      <c r="AN139" s="13"/>
-      <c r="AO139" s="13"/>
-      <c r="AP139" s="13"/>
-      <c r="AQ139" s="13"/>
-      <c r="AR139" s="13"/>
-      <c r="AS139" s="13"/>
-      <c r="AT139" s="13"/>
-      <c r="AU139" s="13"/>
-      <c r="AV139" s="13"/>
-      <c r="AW139" s="13"/>
-      <c r="AX139" s="13"/>
-      <c r="AY139" s="13"/>
-      <c r="AZ139" s="13"/>
-      <c r="BA139" s="13"/>
-      <c r="BB139" s="13"/>
-      <c r="BC139" s="13"/>
-    </row>
-    <row r="140" spans="1:55">
-      <c r="A140" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="B140" s="13"/>
-      <c r="C140" s="13"/>
-      <c r="D140" s="13"/>
-      <c r="E140" s="13"/>
-      <c r="F140" s="13"/>
-      <c r="G140" s="13"/>
-      <c r="H140" s="13"/>
-      <c r="I140" s="13"/>
-      <c r="J140" s="13"/>
-      <c r="K140" s="13"/>
-      <c r="L140" s="13"/>
-      <c r="M140" s="13"/>
-      <c r="N140" s="13"/>
-      <c r="O140" s="13"/>
-      <c r="P140" s="13"/>
-      <c r="Q140" s="13"/>
-      <c r="R140" s="13"/>
-      <c r="S140" s="13"/>
-      <c r="T140" s="13"/>
-      <c r="U140" s="13"/>
-      <c r="V140" s="13"/>
-      <c r="W140" s="13"/>
-      <c r="X140" s="13"/>
-      <c r="Y140" s="13"/>
-      <c r="Z140" s="13"/>
-      <c r="AA140" s="13"/>
-      <c r="AB140" s="13"/>
-      <c r="AC140" s="13"/>
-      <c r="AD140" s="13"/>
-      <c r="AE140" s="13"/>
-      <c r="AF140" s="13"/>
-      <c r="AG140" s="13"/>
-      <c r="AH140" s="13"/>
-      <c r="AI140" s="13"/>
-      <c r="AJ140" s="13"/>
-      <c r="AK140" s="13"/>
-      <c r="AL140" s="13"/>
-      <c r="AM140" s="13"/>
-      <c r="AN140" s="13"/>
-      <c r="AO140" s="13"/>
-      <c r="AP140" s="13"/>
-      <c r="AQ140" s="13"/>
-      <c r="AR140" s="13"/>
-      <c r="AS140" s="13"/>
-      <c r="AT140" s="13"/>
-      <c r="AU140" s="13"/>
-      <c r="AV140" s="13"/>
-      <c r="AW140" s="13"/>
-      <c r="AX140" s="13"/>
-      <c r="AY140" s="13"/>
-      <c r="AZ140" s="13"/>
-      <c r="BA140" s="13"/>
-      <c r="BB140" s="13"/>
-      <c r="BC140" s="13"/>
-    </row>
-    <row r="141" spans="1:55">
-      <c r="A141" s="13" t="s">
-        <v>246</v>
-      </c>
-      <c r="B141" s="13"/>
-      <c r="C141" s="13"/>
-      <c r="D141" s="13"/>
-      <c r="E141" s="13"/>
-      <c r="F141" s="13"/>
-      <c r="G141" s="13"/>
-      <c r="H141" s="13"/>
-      <c r="I141" s="13"/>
-      <c r="J141" s="13"/>
-      <c r="K141" s="13"/>
-      <c r="L141" s="13"/>
-      <c r="M141" s="13"/>
-      <c r="N141" s="13"/>
-      <c r="O141" s="13"/>
-      <c r="P141" s="13"/>
-      <c r="Q141" s="13"/>
-      <c r="R141" s="13"/>
-      <c r="S141" s="13"/>
-      <c r="T141" s="13"/>
-      <c r="U141" s="13"/>
-      <c r="V141" s="13"/>
-      <c r="W141" s="13"/>
-      <c r="X141" s="13"/>
-      <c r="Y141" s="13"/>
-      <c r="Z141" s="13"/>
-      <c r="AA141" s="13"/>
-      <c r="AB141" s="13"/>
-      <c r="AC141" s="13"/>
-      <c r="AD141" s="13"/>
-      <c r="AE141" s="13"/>
-      <c r="AF141" s="13"/>
-      <c r="AG141" s="13"/>
-      <c r="AH141" s="13"/>
-      <c r="AI141" s="13"/>
-      <c r="AJ141" s="13"/>
-      <c r="AK141" s="13"/>
-      <c r="AL141" s="13"/>
-      <c r="AM141" s="13"/>
-      <c r="AN141" s="13"/>
-      <c r="AO141" s="13"/>
-      <c r="AP141" s="13"/>
-      <c r="AQ141" s="13"/>
-      <c r="AR141" s="13"/>
-      <c r="AS141" s="13"/>
-      <c r="AT141" s="13"/>
-      <c r="AU141" s="13"/>
-      <c r="AV141" s="13"/>
-      <c r="AW141" s="13"/>
-      <c r="AX141" s="13"/>
-      <c r="AY141" s="13"/>
-      <c r="AZ141" s="13"/>
-      <c r="BA141" s="13"/>
-      <c r="BB141" s="13"/>
-      <c r="BC141" s="13"/>
-    </row>
-    <row r="142" spans="1:55">
-      <c r="A142" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="B142" s="13"/>
-      <c r="C142" s="13"/>
-      <c r="D142" s="13"/>
-      <c r="E142" s="13"/>
-      <c r="F142" s="13"/>
-      <c r="G142" s="13"/>
-      <c r="H142" s="13"/>
-      <c r="I142" s="13"/>
-      <c r="J142" s="13"/>
-      <c r="K142" s="13"/>
-      <c r="L142" s="13"/>
-      <c r="M142" s="13"/>
-      <c r="N142" s="13"/>
-      <c r="O142" s="13"/>
-      <c r="P142" s="13"/>
-      <c r="Q142" s="13"/>
-      <c r="R142" s="13"/>
-      <c r="S142" s="13"/>
-      <c r="T142" s="13"/>
-      <c r="U142" s="13"/>
-      <c r="V142" s="13"/>
-      <c r="W142" s="13"/>
-      <c r="X142" s="13"/>
-      <c r="Y142" s="13"/>
-      <c r="Z142" s="13"/>
-      <c r="AA142" s="13"/>
-      <c r="AB142" s="13"/>
-      <c r="AC142" s="13"/>
-      <c r="AD142" s="13"/>
-      <c r="AE142" s="13"/>
-      <c r="AF142" s="13"/>
-      <c r="AG142" s="13"/>
-      <c r="AH142" s="13"/>
-      <c r="AI142" s="13"/>
-      <c r="AJ142" s="13"/>
-      <c r="AK142" s="13"/>
-      <c r="AL142" s="13"/>
-      <c r="AM142" s="13"/>
-      <c r="AN142" s="13"/>
-      <c r="AO142" s="13"/>
-      <c r="AP142" s="13"/>
-      <c r="AQ142" s="13"/>
-      <c r="AR142" s="13"/>
-      <c r="AS142" s="13"/>
-      <c r="AT142" s="13"/>
-      <c r="AU142" s="13"/>
-      <c r="AV142" s="13"/>
-      <c r="AW142" s="13"/>
-      <c r="AX142" s="13"/>
-      <c r="AY142" s="13"/>
-      <c r="AZ142" s="13"/>
-      <c r="BA142" s="13"/>
-      <c r="BB142" s="13"/>
-      <c r="BC142" s="13"/>
-    </row>
-    <row r="146" ht="28.8" spans="1:55">
-      <c r="A146" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="B146" s="14"/>
-      <c r="C146" s="14"/>
-      <c r="D146" s="14"/>
-      <c r="E146" s="14"/>
-      <c r="F146" s="14"/>
-      <c r="G146" s="14"/>
-      <c r="H146" s="14"/>
-      <c r="I146" s="14"/>
-      <c r="J146" s="14"/>
-      <c r="K146" s="14"/>
-      <c r="L146" s="14"/>
-      <c r="M146" s="14"/>
-      <c r="N146" s="14"/>
-      <c r="O146" s="14"/>
-      <c r="P146" s="14"/>
-      <c r="Q146" s="14"/>
-      <c r="R146" s="14"/>
-      <c r="S146" s="14"/>
-      <c r="T146" s="14"/>
-      <c r="U146" s="14"/>
-      <c r="V146" s="14"/>
-      <c r="W146" s="14"/>
-      <c r="X146" s="14"/>
-      <c r="Y146" s="14"/>
-      <c r="Z146" s="14"/>
-      <c r="AA146" s="14"/>
-      <c r="AB146" s="14"/>
-      <c r="AC146" s="14"/>
-      <c r="AD146" s="14"/>
-      <c r="AE146" s="14"/>
-      <c r="AF146" s="14"/>
-      <c r="AG146" s="14"/>
-      <c r="AH146" s="14"/>
-      <c r="AI146" s="14"/>
-      <c r="AJ146" s="14"/>
-      <c r="AK146" s="14"/>
-      <c r="AL146" s="14"/>
-      <c r="AM146" s="14"/>
-      <c r="AN146" s="14"/>
-      <c r="AO146" s="14"/>
-      <c r="AP146" s="14"/>
-      <c r="AQ146" s="14"/>
-      <c r="AR146" s="14"/>
-      <c r="AS146" s="14"/>
-      <c r="AT146" s="14"/>
-      <c r="AU146" s="14"/>
-      <c r="AV146" s="14"/>
-      <c r="AW146" s="14"/>
-      <c r="AX146" s="14"/>
-      <c r="AY146" s="14"/>
-      <c r="AZ146" s="14"/>
-      <c r="BA146" s="14"/>
-      <c r="BB146" s="14"/>
-      <c r="BC146" s="14"/>
-    </row>
-    <row r="147" spans="1:55">
-      <c r="A147" s="13" t="s">
-        <v>249</v>
-      </c>
-      <c r="B147" s="13"/>
-      <c r="C147" s="13"/>
-      <c r="D147" s="13"/>
-      <c r="E147" s="13"/>
-      <c r="F147" s="13"/>
-      <c r="G147" s="13"/>
-      <c r="H147" s="13"/>
-      <c r="I147" s="13"/>
-      <c r="J147" s="13"/>
-      <c r="K147" s="13"/>
-      <c r="L147" s="13"/>
-      <c r="M147" s="13"/>
-      <c r="N147" s="13"/>
-      <c r="O147" s="13"/>
-      <c r="P147" s="13"/>
-      <c r="Q147" s="13"/>
-      <c r="R147" s="13"/>
-      <c r="S147" s="13"/>
-      <c r="T147" s="13"/>
-      <c r="U147" s="13"/>
-      <c r="V147" s="13"/>
-      <c r="W147" s="13"/>
-      <c r="X147" s="13"/>
-      <c r="Y147" s="13"/>
-      <c r="Z147" s="13"/>
-      <c r="AA147" s="13"/>
-      <c r="AB147" s="13"/>
-      <c r="AC147" s="13"/>
-      <c r="AD147" s="13"/>
-      <c r="AE147" s="13"/>
-      <c r="AF147" s="13"/>
-      <c r="AG147" s="13"/>
-      <c r="AH147" s="13"/>
-      <c r="AI147" s="13"/>
-      <c r="AJ147" s="13"/>
-      <c r="AK147" s="13"/>
-      <c r="AL147" s="13"/>
-      <c r="AM147" s="13"/>
-      <c r="AN147" s="13"/>
-      <c r="AO147" s="13"/>
-      <c r="AP147" s="13"/>
-      <c r="AQ147" s="13"/>
-      <c r="AR147" s="13"/>
-      <c r="AS147" s="13"/>
-      <c r="AT147" s="13"/>
-      <c r="AU147" s="13"/>
-      <c r="AV147" s="13"/>
-      <c r="AW147" s="13"/>
-      <c r="AX147" s="13"/>
-      <c r="AY147" s="13"/>
-      <c r="AZ147" s="13"/>
-      <c r="BA147" s="13"/>
-      <c r="BB147" s="13"/>
-      <c r="BC147" s="13"/>
-    </row>
-    <row r="148" spans="1:55">
-      <c r="A148" s="13" t="s">
-        <v>250</v>
-      </c>
-      <c r="B148" s="13"/>
-      <c r="C148" s="13"/>
-      <c r="D148" s="13"/>
-      <c r="E148" s="13"/>
-      <c r="F148" s="13"/>
-      <c r="G148" s="13"/>
-      <c r="H148" s="13"/>
-      <c r="I148" s="13"/>
-      <c r="J148" s="13"/>
-      <c r="K148" s="13"/>
-      <c r="L148" s="13"/>
-      <c r="M148" s="13"/>
-      <c r="N148" s="13"/>
-      <c r="O148" s="13"/>
-      <c r="P148" s="13"/>
-      <c r="Q148" s="13"/>
-      <c r="R148" s="13"/>
-      <c r="S148" s="13"/>
-      <c r="T148" s="13"/>
-      <c r="U148" s="13"/>
-      <c r="V148" s="13"/>
-      <c r="W148" s="13"/>
-      <c r="X148" s="13"/>
-      <c r="Y148" s="13"/>
-      <c r="Z148" s="13"/>
-      <c r="AA148" s="13"/>
-      <c r="AB148" s="13"/>
-      <c r="AC148" s="13"/>
-      <c r="AD148" s="13"/>
-      <c r="AE148" s="13"/>
-      <c r="AF148" s="13"/>
-      <c r="AG148" s="13"/>
-      <c r="AH148" s="13"/>
-      <c r="AI148" s="13"/>
-      <c r="AJ148" s="13"/>
-      <c r="AK148" s="13"/>
-      <c r="AL148" s="13"/>
-      <c r="AM148" s="13"/>
-      <c r="AN148" s="13"/>
-      <c r="AO148" s="13"/>
-      <c r="AP148" s="13"/>
-      <c r="AQ148" s="13"/>
-      <c r="AR148" s="13"/>
-      <c r="AS148" s="13"/>
-      <c r="AT148" s="13"/>
-      <c r="AU148" s="13"/>
-      <c r="AV148" s="13"/>
-      <c r="AW148" s="13"/>
-      <c r="AX148" s="13"/>
-      <c r="AY148" s="13"/>
-      <c r="AZ148" s="13"/>
-      <c r="BA148" s="13"/>
-      <c r="BB148" s="13"/>
-      <c r="BC148" s="13"/>
-    </row>
-    <row r="149" spans="1:55">
-      <c r="A149" s="15" t="s">
-        <v>251</v>
-      </c>
-      <c r="B149" s="15"/>
-      <c r="C149" s="15"/>
-      <c r="D149" s="15"/>
-      <c r="E149" s="15"/>
-      <c r="F149" s="15"/>
-      <c r="G149" s="15"/>
-      <c r="H149" s="15"/>
-      <c r="I149" s="15"/>
-      <c r="J149" s="15"/>
-      <c r="K149" s="15"/>
-      <c r="L149" s="15"/>
-      <c r="M149" s="15"/>
-      <c r="N149" s="15"/>
-      <c r="O149" s="15"/>
-      <c r="P149" s="15"/>
-      <c r="Q149" s="15"/>
-      <c r="R149" s="15"/>
-      <c r="S149" s="15"/>
-      <c r="T149" s="15"/>
-      <c r="U149" s="15"/>
-      <c r="V149" s="15"/>
-      <c r="W149" s="15"/>
-      <c r="X149" s="15"/>
-      <c r="Y149" s="15"/>
-      <c r="Z149" s="15"/>
-      <c r="AA149" s="15"/>
-      <c r="AB149" s="15"/>
-      <c r="AC149" s="15"/>
-      <c r="AD149" s="15"/>
-      <c r="AE149" s="15"/>
-      <c r="AF149" s="15"/>
-      <c r="AG149" s="15"/>
-      <c r="AH149" s="15"/>
-      <c r="AI149" s="15"/>
-      <c r="AJ149" s="15"/>
-      <c r="AK149" s="15"/>
-      <c r="AL149" s="15"/>
-      <c r="AM149" s="15"/>
-      <c r="AN149" s="15"/>
-      <c r="AO149" s="15"/>
-      <c r="AP149" s="15"/>
-      <c r="AQ149" s="15"/>
-      <c r="AR149" s="15"/>
-      <c r="AS149" s="15"/>
-      <c r="AT149" s="15"/>
-      <c r="AU149" s="15"/>
-      <c r="AV149" s="15"/>
-      <c r="AW149" s="15"/>
-      <c r="AX149" s="15"/>
-      <c r="AY149" s="15"/>
-      <c r="AZ149" s="15"/>
-      <c r="BA149" s="15"/>
-      <c r="BB149" s="15"/>
-      <c r="BC149" s="15"/>
-    </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="B107:Q107"/>
-    <mergeCell ref="B108:D108"/>
-    <mergeCell ref="G108:I108"/>
-    <mergeCell ref="B118:D118"/>
-    <mergeCell ref="G118:I118"/>
-    <mergeCell ref="B129:D129"/>
-    <mergeCell ref="A138:BC138"/>
-    <mergeCell ref="A139:BC139"/>
-    <mergeCell ref="A140:BC140"/>
-    <mergeCell ref="A141:BC141"/>
-    <mergeCell ref="A142:BC142"/>
-    <mergeCell ref="A146:BC146"/>
-    <mergeCell ref="A147:BC147"/>
-    <mergeCell ref="A148:BC148"/>
-    <mergeCell ref="A149:BC149"/>
-  </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" display="DNA"/>
     <hyperlink ref="F3" r:id="rId2" display="DNA"/>

</xml_diff>